<commit_message>
adaugare interfata de afisat loguri
</commit_message>
<xml_diff>
--- a/src/test/java/com/totsy/xls/Check out.xlsx
+++ b/src/test/java/com/totsy/xls/Check out.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="389">
   <si>
     <t>TCID</t>
   </si>
@@ -1262,6 +1262,104 @@
 Session ID: b2427f6b95d8bcb23838bdd3bd21aeba
 *** Element info: {Using=xpath, value=//ul[@id='header-advertiser_listbox']/li[text()[contains(.,'SANITARIUM')]]}</t>
   </si>
+  <si>
+    <t>FAIL - Could not select Agency from list. no such element: Unable to locate element: {"method":"css selector","selector":"#header-agency-listBox &gt; span &gt; span.k-select &gt; span"}
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: a1cdb60ea38579844ef337114ad8c402
+*** Element info: {Using=css selector, value=#header-agency-listBox &gt; span &gt; span.k-select &gt; span}</t>
+  </si>
+  <si>
+    <t>FAILUnable to select sanit advno such element: Unable to locate element: {"method":"xpath","selector":"//ul[@id='header-advertiser_listbox']/li[text()[contains(.,'SANITARIUM')]]"}
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: a1cdb60ea38579844ef337114ad8c402
+*** Element info: {Using=xpath, value=//ul[@id='header-advertiser_listbox']/li[text()[contains(.,'SANITARIUM')]]}</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on Buttonchrome not reachable
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: 199d5de1d6c94c696c63ab38063b03ca
+*** Element info: {Using=xpath, value=//*[@id="proposals-ref"]}</t>
+  </si>
+  <si>
+    <t>FAIL -- Not able to click on Buttonchrome not reachable
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: 199d5de1d6c94c696c63ab38063b03ca
+*** Element info: {Using=xpath, value=//*[@id="proposals-add"]}</t>
+  </si>
+  <si>
+    <t>FAIL - Could not select Agency from list. chrome not reachable
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: 199d5de1d6c94c696c63ab38063b03ca
+*** Element info: {Using=css selector, value=#header-agency-listBox &gt; span &gt; span.k-select &gt; span}</t>
+  </si>
+  <si>
+    <t>FAIL - Could not select Adv from list. chrome not reachable
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: 199d5de1d6c94c696c63ab38063b03ca
+*** Element info: {Using=css selector, value=#header-advertiser-listBox &gt; span &gt; span.k-select &gt; span}</t>
+  </si>
+  <si>
+    <t>FAIL - Could not select Agency from list. no such element: Unable to locate element: {"method":"css selector","selector":"#header-agency-listBox &gt; span &gt; span.k-select &gt; span"}
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: 54a8f162a8f804c64d4a09a66658c76e
+*** Element info: {Using=css selector, value=#header-agency-listBox &gt; span &gt; span.k-select &gt; span}</t>
+  </si>
+  <si>
+    <t>FAILUnable to select sanit advelement not visible
+  (Session info: chrome=64.0.3282.186)
+  (Driver info: chromedriver=2.35.528161 (5b82f2d2aae0ca24b877009200ced9065a772e73),platform=Windows NT 10.0.16299 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 0 milliseconds
+Build info: version: '3.9.1', revision: '63f7b50', time: '2018-02-07T22:42:28.403Z'
+System info: host: 'DESKTOP-J8SME32', ip: '192.168.100.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, acceptSslCerts: false, applicationCacheEnabled: false, browserConnectionEnabled: false, browserName: chrome, chrome: {chromedriverVersion: 2.35.528161 (5b82f2d2aae0ca..., userDataDir: C:\Users\Iulian\AppData\Loc...}, cssSelectorsEnabled: true, databaseEnabled: false, handlesAlerts: true, hasTouchScreen: false, javascriptEnabled: true, locationContextEnabled: true, mobileEmulationEnabled: false, nativeEvents: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: XP, platformName: XP, rotatable: false, setWindowRect: true, takesHeapSnapshot: true, takesScreenshot: true, unexpectedAlertBehaviour: , unhandledPromptBehavior: , version: 64.0.3282.186, webStorageEnabled: true}
+Session ID: 54a8f162a8f804c64d4a09a66658c76e</t>
+  </si>
 </sst>
 </file>
 
@@ -1270,7 +1368,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2017,10 +2115,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="37.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="23.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="37.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2192,22 +2290,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="18.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" style="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" style="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" style="16" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="78.7109375" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="10.42578125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="16" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="16" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="16" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="16" width="16.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="16" width="19.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="16" width="9.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="16" width="15.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="16" width="6.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="16" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="16" width="5.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="16" width="9.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="16" width="78.7109375" collapsed="true"/>
+    <col min="17" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -2776,23 +2874,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="6.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" style="16" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="78.7109375" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="20.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="6.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="16" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="16" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="16" width="16.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="16" width="16.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="16" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="16" width="15.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="16" width="6.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="16" width="18.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="16" width="78.7109375" collapsed="true"/>
+    <col min="17" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -3360,22 +3458,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15" style="16" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="255" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="17.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="20.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="6.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="16" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="16" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="16" width="16.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="16" width="16.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="16" width="11.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="16" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="16" width="6.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="16" width="18.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="16" width="255.0" collapsed="true"/>
+    <col min="16" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -3910,23 +4008,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="18.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13" style="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.7109375" style="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15" style="16" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="29.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="78.7109375" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="10.42578125" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="16" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="16" width="13.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="16" width="15.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="16" width="16.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="16" width="19.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="16" width="9.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="16" width="15.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="16" width="6.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="16" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="16" width="5.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="16" width="29.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="16" width="9.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="16" width="78.7109375" collapsed="true"/>
+    <col min="18" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -4527,19 +4625,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="2" collapsed="1"/>
-    <col min="3" max="3" width="27.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="255" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="16" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="8.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" style="2" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="27.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="20.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="36.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="24.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="255.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="255.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="255.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="7.51171875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="8.62890625" collapsed="true"/>
+    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5110,7 +5213,7 @@
       </c>
       <c r="G12" s="9"/>
       <c r="H12" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="I12" t="s">
         <v>267</v>
@@ -5210,7 +5313,7 @@
       </c>
       <c r="G14" s="9"/>
       <c r="H14" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="I14" t="s">
         <v>267</v>
@@ -13431,10 +13534,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="61.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="18.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="61.85546875" collapsed="true"/>
+    <col min="4" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -13606,9 +13709,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="3" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -13714,10 +13817,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="255" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="16" width="255.0" collapsed="true"/>
+    <col min="4" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -13845,12 +13948,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="50.7109375" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="255" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="50.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="16" width="255.0" collapsed="true"/>
+    <col min="6" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -14038,10 +14141,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="255" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="16" width="255.0" collapsed="true"/>
+    <col min="4" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -14169,17 +14272,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="255" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="16" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="16" width="11.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="16" width="18.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="16" width="255.0" collapsed="true"/>
+    <col min="11" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -14549,17 +14652,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" style="16" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="16" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.85546875" style="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7" style="16" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.5703125" style="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="255" style="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.140625" style="16" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="11.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="16" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="16" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="16" width="16.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="16" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="16" width="11.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="16" width="18.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="16" width="7.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="16" width="9.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="16" width="255.0" collapsed="true"/>
+    <col min="11" max="16384" style="16" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>